<commit_message>
Final Draft complete 🐱‍�ð±‍🏍
</commit_message>
<xml_diff>
--- a/Paperwork/Final Paper/timing.xlsx
+++ b/Paperwork/Final Paper/timing.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rptal\Documents\School\Honors-Thesis\Paperwork\Final Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064758BA-5B4F-4737-9DBE-F2343FBE43B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F548A97-93A2-4089-ADD7-4B6DEED3FF02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1222" yWindow="-98" windowWidth="22876" windowHeight="13695" xr2:uid="{04790142-B22C-4A9C-A341-F4FB163EB50A}"/>
+    <workbookView xWindow="1200" yWindow="-120" windowWidth="27720" windowHeight="16440" xr2:uid="{04790142-B22C-4A9C-A341-F4FB163EB50A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>iPhone XS</t>
   </si>
@@ -65,6 +64,9 @@
   </si>
   <si>
     <t>stdd</t>
+  </si>
+  <si>
+    <t>peak performance</t>
   </si>
 </sst>
 </file>
@@ -416,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45123E19-5586-4C37-A4FF-52B08BB817E9}">
-  <dimension ref="A3:J49"/>
+  <dimension ref="A3:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +433,7 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -450,8 +452,17 @@
       <c r="J3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -476,8 +487,20 @@
       <c r="J4">
         <v>242.738709</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>69.334958999999998</v>
+      </c>
+      <c r="N4">
+        <v>172.47475</v>
+      </c>
+      <c r="O4">
+        <v>270.01920799999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>4.2500830000000001</v>
       </c>
@@ -496,8 +519,20 @@
       <c r="J5">
         <v>274.07175000000001</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5">
+        <v>68.317542000000003</v>
+      </c>
+      <c r="N5">
+        <v>171.12154200000001</v>
+      </c>
+      <c r="O5">
+        <v>274.99041599999998</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>5.333583</v>
       </c>
@@ -516,8 +551,17 @@
       <c r="J6">
         <v>253.53358399999999</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>68.810708000000005</v>
+      </c>
+      <c r="N6">
+        <v>163.882417</v>
+      </c>
+      <c r="O6">
+        <v>269.14495899999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>24.561416000000001</v>
       </c>
@@ -536,8 +580,17 @@
       <c r="J7">
         <v>277.20012500000001</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>66.476624999999999</v>
+      </c>
+      <c r="N7">
+        <v>134.31899999999999</v>
+      </c>
+      <c r="O7">
+        <v>268.80212499999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>22.863458000000001</v>
       </c>
@@ -556,8 +609,17 @@
       <c r="J8">
         <v>261.70637499999998</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>59.403584000000002</v>
+      </c>
+      <c r="N8">
+        <v>167.44483399999999</v>
+      </c>
+      <c r="O8">
+        <v>250.07070899999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>20.345124999999999</v>
       </c>
@@ -576,8 +638,17 @@
       <c r="J9">
         <v>249.966667</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>68.381249999999994</v>
+      </c>
+      <c r="N9">
+        <v>139.61366699999999</v>
+      </c>
+      <c r="O9">
+        <v>254.253041</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>24.279125000000001</v>
       </c>
@@ -596,8 +667,17 @@
       <c r="J10">
         <v>265.31841600000001</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>59.845458999999998</v>
+      </c>
+      <c r="N10">
+        <v>170.199333</v>
+      </c>
+      <c r="O10">
+        <v>274.74308300000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>14.198582999999999</v>
       </c>
@@ -616,8 +696,17 @@
       <c r="J11">
         <v>250.97662500000001</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>67.410291999999998</v>
+      </c>
+      <c r="N11">
+        <v>134.09899999999999</v>
+      </c>
+      <c r="O11">
+        <v>271.212625</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>23.222291999999999</v>
       </c>
@@ -636,8 +725,17 @@
       <c r="J12">
         <v>230.1755</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>54.477666999999997</v>
+      </c>
+      <c r="N12">
+        <v>169.280542</v>
+      </c>
+      <c r="O12">
+        <v>268.065292</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>23.153915999999999</v>
       </c>
@@ -656,8 +754,17 @@
       <c r="J13">
         <v>273.62112500000001</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>68.938374999999994</v>
+      </c>
+      <c r="N13">
+        <v>176.09141700000001</v>
+      </c>
+      <c r="O13">
+        <v>274.78004099999998</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>20.610624999999999</v>
       </c>
@@ -676,8 +783,17 @@
       <c r="J14">
         <v>271.272583</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>65.141499999999994</v>
+      </c>
+      <c r="N14">
+        <v>136.46674999999999</v>
+      </c>
+      <c r="O14">
+        <v>259.22149999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>23.774042000000001</v>
       </c>
@@ -696,8 +812,17 @@
       <c r="J15">
         <v>258.72870799999998</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>67.759165999999993</v>
+      </c>
+      <c r="N15">
+        <v>162.540167</v>
+      </c>
+      <c r="O15">
+        <v>255.53895800000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>22.413333000000002</v>
       </c>
@@ -716,8 +841,17 @@
       <c r="J16">
         <v>233.81762499999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>68.075249999999997</v>
+      </c>
+      <c r="N16">
+        <v>169.446459</v>
+      </c>
+      <c r="O16">
+        <v>257.33108399999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>19.759625</v>
       </c>
@@ -736,8 +870,17 @@
       <c r="J17">
         <v>265.49195800000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>67.967958999999993</v>
+      </c>
+      <c r="N17">
+        <v>166.809</v>
+      </c>
+      <c r="O17">
+        <v>261.83550000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>23.056833000000001</v>
       </c>
@@ -756,8 +899,17 @@
       <c r="J18">
         <v>263.912667</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>64.070041000000003</v>
+      </c>
+      <c r="N18">
+        <v>135.40375</v>
+      </c>
+      <c r="O18">
+        <v>226.20762500000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>19.705625000000001</v>
       </c>
@@ -776,8 +928,17 @@
       <c r="J19">
         <v>252.119708</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>64.549333000000004</v>
+      </c>
+      <c r="N19">
+        <v>161.56908300000001</v>
+      </c>
+      <c r="O19">
+        <v>262.657917</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>21.213417</v>
       </c>
@@ -796,8 +957,17 @@
       <c r="J20">
         <v>273.64262500000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>68.817082999999997</v>
+      </c>
+      <c r="N20">
+        <v>174.80808300000001</v>
+      </c>
+      <c r="O20">
+        <v>269.58195799999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>22.476375000000001</v>
       </c>
@@ -816,8 +986,17 @@
       <c r="J21">
         <v>284.07883399999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>61.627791999999999</v>
+      </c>
+      <c r="N21">
+        <v>148.61125000000001</v>
+      </c>
+      <c r="O21">
+        <v>263.39675</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>22.954249999999998</v>
       </c>
@@ -836,8 +1015,17 @@
       <c r="J22">
         <v>248.620541</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>69.566374999999994</v>
+      </c>
+      <c r="N22">
+        <v>137.03508400000001</v>
+      </c>
+      <c r="O22">
+        <v>263.07612499999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>19.944666000000002</v>
       </c>
@@ -856,8 +1044,17 @@
       <c r="J23">
         <v>268.60279100000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>69.552750000000003</v>
+      </c>
+      <c r="N23">
+        <v>159.09679199999999</v>
+      </c>
+      <c r="O23">
+        <v>266.82570900000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -885,8 +1082,20 @@
         <f t="shared" ref="J24" si="3">AVERAGE(J4:J23)</f>
         <v>259.97984580000008</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <f t="shared" ref="M24:O24" si="4">AVERAGE(M4:M23)</f>
+        <v>65.926185499999988</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="4"/>
+        <v>157.515646</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="4"/>
+        <v>263.08773124999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -895,27 +1104,39 @@
         <v>5.5311629901224038</v>
       </c>
       <c r="D25">
-        <f t="shared" ref="D25:J25" si="4">_xlfn.STDEV.S(D4:D24)</f>
+        <f t="shared" ref="D25:J25" si="5">_xlfn.STDEV.S(D4:D24)</f>
         <v>9.1978264354292989</v>
       </c>
       <c r="E25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.4816616315384934</v>
       </c>
       <c r="H25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.9993854242433287</v>
       </c>
       <c r="I25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11.094436294911022</v>
       </c>
       <c r="J25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.165317519429927</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <f t="shared" ref="M25:O25" si="6">_xlfn.STDEV.S(M4:M24)</f>
+        <v>4.032328128524072</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="6"/>
+        <v>15.168917563928202</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="6"/>
+        <v>10.93872569141584</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>7</v>
       </c>
@@ -923,17 +1144,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C28">
-        <f>C4/2</f>
+        <f t="shared" ref="C28:C47" si="7">C4/2</f>
         <v>9.3858955000000002</v>
       </c>
       <c r="D28">
-        <f>D4/5</f>
+        <f t="shared" ref="D28:D47" si="8">D4/5</f>
         <v>10.7902916</v>
       </c>
       <c r="E28">
-        <f>E4/8</f>
+        <f t="shared" ref="E28:E47" si="9">E4/8</f>
         <v>9.8955416249999999</v>
       </c>
       <c r="H28">
@@ -948,502 +1169,742 @@
         <f>J4/8</f>
         <v>30.342338625</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <f>M4/2</f>
+        <v>34.667479499999999</v>
+      </c>
+      <c r="N28">
+        <f>N4/5</f>
+        <v>34.494950000000003</v>
+      </c>
+      <c r="O28">
+        <f>O4/8</f>
+        <v>33.752400999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C29">
-        <f>C5/2</f>
+        <f t="shared" si="7"/>
         <v>2.1250415</v>
       </c>
       <c r="D29">
-        <f>D5/5</f>
+        <f t="shared" si="8"/>
         <v>10.717241599999999</v>
       </c>
       <c r="E29">
-        <f>E5/8</f>
+        <f t="shared" si="9"/>
         <v>9.5460364999999996</v>
       </c>
       <c r="H29">
-        <f t="shared" ref="H29:H47" si="5">H5/2</f>
+        <f t="shared" ref="H29:H47" si="10">H5/2</f>
         <v>30.641500000000001</v>
       </c>
       <c r="I29">
-        <f t="shared" ref="I29:I47" si="6">I5/5</f>
+        <f t="shared" ref="I29:I47" si="11">I5/5</f>
         <v>37.399633199999997</v>
       </c>
       <c r="J29">
-        <f t="shared" ref="J29:J47" si="7">J5/8</f>
+        <f t="shared" ref="J29:O47" si="12">J5/8</f>
         <v>34.258968750000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <f t="shared" ref="M29:M47" si="13">M5/2</f>
+        <v>34.158771000000002</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ref="N29:N47" si="14">N5/5</f>
+        <v>34.224308399999998</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ref="O29:O47" si="15">O5/8</f>
+        <v>34.373801999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C30">
-        <f>C6/2</f>
+        <f t="shared" si="7"/>
         <v>2.6667915</v>
       </c>
       <c r="D30">
-        <f>D6/5</f>
+        <f t="shared" si="8"/>
         <v>5.9460084000000002</v>
       </c>
       <c r="E30">
-        <f>E6/8</f>
+        <f t="shared" si="9"/>
         <v>9.5178646249999996</v>
       </c>
       <c r="H30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>34.046833499999998</v>
       </c>
       <c r="I30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>32.979483399999999</v>
       </c>
       <c r="J30">
+        <f t="shared" si="12"/>
+        <v>31.691697999999999</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="13"/>
+        <v>34.405354000000003</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="14"/>
+        <v>32.776483400000004</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="15"/>
+        <v>33.643119874999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C31">
         <f t="shared" si="7"/>
-        <v>31.691697999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <f>C7/2</f>
         <v>12.280708000000001</v>
       </c>
       <c r="D31">
-        <f>D7/5</f>
+        <f t="shared" si="8"/>
         <v>9.8637332000000004</v>
       </c>
       <c r="E31">
-        <f>E7/8</f>
+        <f t="shared" si="9"/>
         <v>8.8888698749999993</v>
       </c>
       <c r="H31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>33.511833000000003</v>
       </c>
       <c r="I31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>34.273683200000001</v>
       </c>
       <c r="J31">
+        <f t="shared" si="12"/>
+        <v>34.650015625000002</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="13"/>
+        <v>33.238312499999999</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="14"/>
+        <v>26.863799999999998</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="15"/>
+        <v>33.600265624999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C32">
         <f t="shared" si="7"/>
-        <v>34.650015625000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C32">
-        <f>C8/2</f>
         <v>11.431729000000001</v>
       </c>
       <c r="D32">
-        <f>D8/5</f>
+        <f t="shared" si="8"/>
         <v>8.9308000000000014</v>
       </c>
       <c r="E32">
-        <f>E8/8</f>
+        <f t="shared" si="9"/>
         <v>10.095177124999999</v>
       </c>
       <c r="H32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>33.4870625</v>
       </c>
       <c r="I32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>31.262341600000003</v>
       </c>
       <c r="J32">
+        <f t="shared" si="12"/>
+        <v>32.713296874999997</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="13"/>
+        <v>29.701792000000001</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="14"/>
+        <v>33.4889668</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="15"/>
+        <v>31.258838624999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C33">
         <f t="shared" si="7"/>
-        <v>32.713296874999997</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C33">
-        <f>C9/2</f>
         <v>10.1725625</v>
       </c>
       <c r="D33">
-        <f>D9/5</f>
+        <f t="shared" si="8"/>
         <v>10.8972584</v>
       </c>
       <c r="E33">
-        <f>E9/8</f>
+        <f t="shared" si="9"/>
         <v>9.1179791249999997</v>
       </c>
       <c r="H33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>26.644978999999999</v>
       </c>
       <c r="I33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>31.890525000000004</v>
       </c>
       <c r="J33">
+        <f t="shared" si="12"/>
+        <v>31.245833375</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="13"/>
+        <v>34.190624999999997</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="14"/>
+        <v>27.922733399999998</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="15"/>
+        <v>31.781630125</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C34">
         <f t="shared" si="7"/>
-        <v>31.245833375</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C34">
-        <f>C10/2</f>
         <v>12.1395625</v>
       </c>
       <c r="D34">
-        <f>D10/5</f>
+        <f t="shared" si="8"/>
         <v>9.7836668000000007</v>
       </c>
       <c r="E34">
-        <f>E10/8</f>
+        <f t="shared" si="9"/>
         <v>9.3120312500000004</v>
       </c>
       <c r="H34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>33.365812499999997</v>
       </c>
       <c r="I34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>34.592541599999997</v>
       </c>
       <c r="J34">
+        <f t="shared" si="12"/>
+        <v>33.164802000000002</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="13"/>
+        <v>29.922729499999999</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="14"/>
+        <v>34.039866599999996</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="15"/>
+        <v>34.342885375000002</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C35">
         <f t="shared" si="7"/>
-        <v>33.164802000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C35">
-        <f>C11/2</f>
         <v>7.0992914999999996</v>
       </c>
       <c r="D35">
-        <f>D11/5</f>
+        <f t="shared" si="8"/>
         <v>10.919866600000001</v>
       </c>
       <c r="E35">
-        <f>E11/8</f>
+        <f t="shared" si="9"/>
         <v>9.2270208749999991</v>
       </c>
       <c r="H35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>28.543208499999999</v>
       </c>
       <c r="I35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>34.632999999999996</v>
       </c>
       <c r="J35">
+        <f t="shared" si="12"/>
+        <v>31.372078125000002</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="13"/>
+        <v>33.705145999999999</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="14"/>
+        <v>26.819799999999997</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="15"/>
+        <v>33.901578125</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C36">
         <f t="shared" si="7"/>
-        <v>31.372078125000002</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C36">
-        <f>C12/2</f>
         <v>11.611146</v>
       </c>
       <c r="D36">
-        <f>D12/5</f>
+        <f t="shared" si="8"/>
         <v>10.522066800000001</v>
       </c>
       <c r="E36">
-        <f>E12/8</f>
+        <f t="shared" si="9"/>
         <v>9.5344582500000001</v>
       </c>
       <c r="H36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>33.5278955</v>
       </c>
       <c r="I36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>30.568116800000002</v>
       </c>
       <c r="J36">
+        <f t="shared" si="12"/>
+        <v>28.7719375</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="13"/>
+        <v>27.238833499999998</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="14"/>
+        <v>33.856108399999997</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="15"/>
+        <v>33.5081615</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C37">
         <f t="shared" si="7"/>
-        <v>28.7719375</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C37">
-        <f>C13/2</f>
         <v>11.576957999999999</v>
       </c>
       <c r="D37">
-        <f>D13/5</f>
+        <f t="shared" si="8"/>
         <v>9.8231166000000005</v>
       </c>
       <c r="E37">
-        <f>E13/8</f>
+        <f t="shared" si="9"/>
         <v>11.221781249999999</v>
       </c>
       <c r="H37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>34.325958499999999</v>
       </c>
       <c r="I37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>30.236049999999999</v>
       </c>
       <c r="J37">
+        <f t="shared" si="12"/>
+        <v>34.202640625000001</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="13"/>
+        <v>34.469187499999997</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="14"/>
+        <v>35.218283400000004</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="15"/>
+        <v>34.347505124999998</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C38">
         <f t="shared" si="7"/>
-        <v>34.202640625000001</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C38">
-        <f>C14/2</f>
         <v>10.305312499999999</v>
       </c>
       <c r="D38">
-        <f>D14/5</f>
+        <f t="shared" si="8"/>
         <v>8.0950999999999986</v>
       </c>
       <c r="E38">
-        <f>E14/8</f>
+        <f t="shared" si="9"/>
         <v>10.2481875</v>
       </c>
       <c r="H38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>30.439146000000001</v>
       </c>
       <c r="I38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>33.700191599999997</v>
       </c>
       <c r="J38">
+        <f t="shared" si="12"/>
+        <v>33.909072875</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="13"/>
+        <v>32.570749999999997</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="14"/>
+        <v>27.293349999999997</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="15"/>
+        <v>32.402687499999999</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C39">
         <f t="shared" si="7"/>
-        <v>33.909072875</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C39">
-        <f>C15/2</f>
         <v>11.887021000000001</v>
       </c>
       <c r="D39">
-        <f>D15/5</f>
+        <f t="shared" si="8"/>
         <v>11.0323916</v>
       </c>
       <c r="E39">
-        <f>E15/8</f>
+        <f t="shared" si="9"/>
         <v>8.9445103750000001</v>
       </c>
       <c r="H39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>34.193979499999998</v>
       </c>
       <c r="I39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>33.714758400000001</v>
       </c>
       <c r="J39">
+        <f t="shared" si="12"/>
+        <v>32.341088499999998</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="13"/>
+        <v>33.879582999999997</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="14"/>
+        <v>32.508033400000002</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="15"/>
+        <v>31.942369750000001</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C40">
         <f t="shared" si="7"/>
-        <v>32.341088499999998</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C40">
-        <f>C16/2</f>
         <v>11.206666500000001</v>
       </c>
       <c r="D40">
-        <f>D16/5</f>
+        <f t="shared" si="8"/>
         <v>9.3685834000000003</v>
       </c>
       <c r="E40">
-        <f>E16/8</f>
+        <f t="shared" si="9"/>
         <v>9.5241144999999996</v>
       </c>
       <c r="H40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>34.181791500000003</v>
       </c>
       <c r="I40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>27.307433200000002</v>
       </c>
       <c r="J40">
+        <f t="shared" si="12"/>
+        <v>29.227203124999999</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="13"/>
+        <v>34.037624999999998</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="14"/>
+        <v>33.889291800000002</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="15"/>
+        <v>32.166385499999997</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C41">
         <f t="shared" si="7"/>
-        <v>29.227203124999999</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C41">
-        <f>C17/2</f>
         <v>9.8798124999999999</v>
       </c>
       <c r="D41">
-        <f>D17/5</f>
+        <f t="shared" si="8"/>
         <v>9.7784665999999998</v>
       </c>
       <c r="E41">
-        <f>E17/8</f>
+        <f t="shared" si="9"/>
         <v>8.4915363750000008</v>
       </c>
       <c r="H41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>33.493333499999999</v>
       </c>
       <c r="I41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>31.629516599999999</v>
       </c>
       <c r="J41">
+        <f t="shared" si="12"/>
+        <v>33.186494750000001</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="13"/>
+        <v>33.983979499999997</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="14"/>
+        <v>33.361800000000002</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="15"/>
+        <v>32.729437500000003</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C42">
         <f t="shared" si="7"/>
-        <v>33.186494750000001</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C42">
-        <f>C18/2</f>
         <v>11.528416500000001</v>
       </c>
       <c r="D42">
-        <f>D18/5</f>
+        <f t="shared" si="8"/>
         <v>3.1462250000000003</v>
       </c>
       <c r="E42">
-        <f>E18/8</f>
+        <f t="shared" si="9"/>
         <v>8.7874009999999991</v>
       </c>
       <c r="H42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>35.802458000000001</v>
       </c>
       <c r="I42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>33.383266599999999</v>
       </c>
       <c r="J42">
+        <f t="shared" si="12"/>
+        <v>32.989083375</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="13"/>
+        <v>32.035020500000002</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="14"/>
+        <v>27.080750000000002</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="15"/>
+        <v>28.275953125000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C43">
         <f t="shared" si="7"/>
-        <v>32.989083375</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C43">
-        <f>C19/2</f>
         <v>9.8528125000000006</v>
       </c>
       <c r="D43">
-        <f>D19/5</f>
+        <f t="shared" si="8"/>
         <v>10.025433400000001</v>
       </c>
       <c r="E43">
-        <f>E19/8</f>
+        <f t="shared" si="9"/>
         <v>9.5733437499999994</v>
       </c>
       <c r="H43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>34.089979499999998</v>
       </c>
       <c r="I43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>32.0206582</v>
       </c>
       <c r="J43">
+        <f t="shared" si="12"/>
+        <v>31.5149635</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="13"/>
+        <v>32.274666500000002</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="14"/>
+        <v>32.313816600000003</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="15"/>
+        <v>32.832239625</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C44">
         <f t="shared" si="7"/>
-        <v>31.5149635</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C44">
-        <f>C20/2</f>
         <v>10.6067085</v>
       </c>
       <c r="D44">
-        <f>D20/5</f>
+        <f t="shared" si="8"/>
         <v>9.7171249999999993</v>
       </c>
       <c r="E44">
-        <f>E20/8</f>
+        <f t="shared" si="9"/>
         <v>9.8902394999999999</v>
       </c>
       <c r="H44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>34.081375000000001</v>
       </c>
       <c r="I44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>35.641258399999998</v>
       </c>
       <c r="J44">
+        <f t="shared" si="12"/>
+        <v>34.205328125000001</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="13"/>
+        <v>34.408541499999998</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="14"/>
+        <v>34.961616599999999</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="15"/>
+        <v>33.697744749999998</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C45">
         <f t="shared" si="7"/>
-        <v>34.205328125000001</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C45">
-        <f>C21/2</f>
         <v>11.2381875</v>
       </c>
       <c r="D45">
-        <f>D21/5</f>
+        <f t="shared" si="8"/>
         <v>8.9728750000000002</v>
       </c>
       <c r="E45">
-        <f>E21/8</f>
+        <f t="shared" si="9"/>
         <v>10.70921875</v>
       </c>
       <c r="H45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>33.664895999999999</v>
       </c>
       <c r="I45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>33.89085</v>
       </c>
       <c r="J45">
+        <f t="shared" si="12"/>
+        <v>35.509854249999997</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="13"/>
+        <v>30.813896</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="14"/>
+        <v>29.722250000000003</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="15"/>
+        <v>32.92459375</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C46">
         <f t="shared" si="7"/>
-        <v>35.509854249999997</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C46">
-        <f>C22/2</f>
         <v>11.477124999999999</v>
       </c>
       <c r="D46">
-        <f>D22/5</f>
+        <f t="shared" si="8"/>
         <v>8.453875</v>
       </c>
       <c r="E46">
-        <f>E22/8</f>
+        <f t="shared" si="9"/>
         <v>9.0710416249999994</v>
       </c>
       <c r="H46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>34.174687499999997</v>
       </c>
       <c r="I46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>32.146541599999999</v>
       </c>
       <c r="J46">
+        <f t="shared" si="12"/>
+        <v>31.077567625</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="13"/>
+        <v>34.783187499999997</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="14"/>
+        <v>27.407016800000001</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="15"/>
+        <v>32.884515624999999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C47">
         <f t="shared" si="7"/>
-        <v>31.077567625</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C47">
-        <f>C23/2</f>
         <v>9.9723330000000008</v>
       </c>
       <c r="D47">
-        <f>D23/5</f>
+        <f t="shared" si="8"/>
         <v>10.02445</v>
       </c>
       <c r="E47">
-        <f>E23/8</f>
+        <f t="shared" si="9"/>
         <v>10.656854125000001</v>
       </c>
       <c r="H47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>29.969687499999999</v>
       </c>
       <c r="I47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>31.941283399999996</v>
       </c>
       <c r="J47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>33.575348875000003</v>
       </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <f t="shared" si="13"/>
+        <v>34.776375000000002</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="14"/>
+        <v>31.819358399999999</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="15"/>
+        <v>33.353213625000002</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>8</v>
       </c>
@@ -1458,8 +1919,12 @@
         <f>AVERAGE(H28:J47)</f>
         <v>32.542818920000009</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <f>AVERAGE(M28:O47)</f>
+        <v>32.45072945208333</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>10</v>
       </c>
@@ -1473,6 +1938,10 @@
       <c r="H49">
         <f>_xlfn.STDEV.S(H28:J47)</f>
         <v>2.203450659837721</v>
+      </c>
+      <c r="M49">
+        <f>_xlfn.STDEV.S(M28:O47)</f>
+        <v>2.364158513045048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>